<commit_message>
Access to the cells in the row
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFCF233-12A0-4D10-8B1A-6AB34D6A9DA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EF5BCE-DC1A-4DE0-A856-C0C0E80EE395}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>